<commit_message>
avg speaker performance graph
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -19,21 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Play</t>
   </si>
   <si>
-    <t>Pruned random F1</t>
+    <t>Random</t>
   </si>
   <si>
-    <t>Pruned most common F1</t>
+    <t>Most Common</t>
   </si>
   <si>
-    <t>Pruned system LIWC F1</t>
+    <t>LogReg LIWC</t>
   </si>
   <si>
-    <t>Pruned system word F1</t>
+    <t>LogReg word</t>
+  </si>
+  <si>
+    <t>Naïve Bayes LIWC</t>
+  </si>
+  <si>
+    <t>kNN LIWC</t>
+  </si>
+  <si>
+    <t>KMeans LIWC</t>
+  </si>
+  <si>
+    <t>Decision Tree LIWC</t>
+  </si>
+  <si>
+    <t>Avg</t>
   </si>
 </sst>
 </file>
@@ -122,10 +137,10 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="5"/>
+          <c:order val="5"/>
           <c:tx>
-            <c:v>Pruned Random</c:v>
+            <c:v>Random</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -369,257 +384,10 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="6"/>
+          <c:order val="6"/>
           <c:tx>
-            <c:v>Pruned Most Common</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.14</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.29</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.38</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Pruned System LIWC</c:v>
+            <c:v>Logistic Regression</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -863,125 +631,1244 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="7"/>
+          <c:order val="7"/>
           <c:tx>
-            <c:v>Pruned System Word</c:v>
+            <c:v>k Means</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$37</c:f>
+              <c:f>Sheet1!$H$2:$H$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>0.76</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.07</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>kNN</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.85</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.99</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.83</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.9</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.87</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.81</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.97</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.71</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.89</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.85</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.81</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.92</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.94</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.97</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.84</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.0</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.82</c:v>
+                  <c:v>0.57</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.71</c:v>
+                  <c:v>0.29</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.97</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.7</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.79</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.97</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.96</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.93</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.94</c:v>
+                  <c:v>0.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Decision Tree</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Random</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="07B5FF"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Logistic Regression</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00A500"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>k Means</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.07</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>kNN</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.29</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Decision Tree</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,11 +1883,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2073802616"/>
-        <c:axId val="2073925272"/>
+        <c:axId val="2069441736"/>
+        <c:axId val="2069444680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2073802616"/>
+        <c:axId val="2069441736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,7 +1897,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073925272"/>
+        <c:crossAx val="2069444680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1018,7 +1905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073925272"/>
+        <c:axId val="2069444680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1059,7 +1946,306 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2073802616"/>
+        <c:crossAx val="2069441736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average classifier speaker prediction performance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>with LIWC features on pruned dataset</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>k Means</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0758333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Decision Tree</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.595555555555555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>kNN</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.531111111111111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Naive Bayes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.341944444444444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Logistic Regression</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.385555555555556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Random</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.166944444444444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Most Common</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.133333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2067920616"/>
+        <c:axId val="2067922888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2067920616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2067922888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2067922888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>F1 Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2067920616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1101,16 +2287,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1124,6 +2310,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1454,21 +2672,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:9" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1484,8 +2703,20 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
+    <row r="2" spans="1:9" ht="16">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1501,8 +2732,20 @@
       <c r="E2" s="2">
         <v>0.76</v>
       </c>
+      <c r="F2" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.51</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="16">
+    <row r="3" spans="1:9" ht="16">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1518,8 +2761,20 @@
       <c r="E3" s="2">
         <v>0.85</v>
       </c>
+      <c r="F3" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.63</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:9" ht="16">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1535,8 +2790,20 @@
       <c r="E4" s="2">
         <v>0.96</v>
       </c>
+      <c r="F4" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="16">
+    <row r="5" spans="1:9" ht="16">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1552,8 +2819,20 @@
       <c r="E5" s="2">
         <v>0.99</v>
       </c>
+      <c r="F5" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.61</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="16">
+    <row r="6" spans="1:9" ht="16">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1569,8 +2848,20 @@
       <c r="E6" s="2">
         <v>0.74</v>
       </c>
+      <c r="F6" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.63</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" ht="16">
+    <row r="7" spans="1:9" ht="16">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1586,8 +2877,20 @@
       <c r="E7" s="2">
         <v>0.96</v>
       </c>
+      <c r="F7" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.47</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" ht="16">
+    <row r="8" spans="1:9" ht="16">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1603,8 +2906,20 @@
       <c r="E8" s="2">
         <v>0.64</v>
       </c>
+      <c r="F8" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.56000000000000005</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" ht="16">
+    <row r="9" spans="1:9" ht="16">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1620,8 +2935,20 @@
       <c r="E9" s="2">
         <v>0.85</v>
       </c>
+      <c r="F9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.77</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
+    <row r="10" spans="1:9" ht="16">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1637,8 +2964,20 @@
       <c r="E10" s="2">
         <v>0.83</v>
       </c>
+      <c r="F10" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.56999999999999995</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" ht="16">
+    <row r="11" spans="1:9" ht="16">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1654,8 +2993,20 @@
       <c r="E11" s="2">
         <v>1</v>
       </c>
+      <c r="F11" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.77</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:9" ht="16">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1671,8 +3022,20 @@
       <c r="E12" s="2">
         <v>0.9</v>
       </c>
+      <c r="F12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" ht="16">
+    <row r="13" spans="1:9" ht="16">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1688,8 +3051,20 @@
       <c r="E13" s="2">
         <v>0.99</v>
       </c>
+      <c r="F13" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:9" ht="16">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1705,8 +3080,20 @@
       <c r="E14" s="2">
         <v>0.87</v>
       </c>
+      <c r="F14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.57999999999999996</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" ht="16">
+    <row r="15" spans="1:9" ht="16">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1722,8 +3109,20 @@
       <c r="E15" s="2">
         <v>0.81</v>
       </c>
+      <c r="F15" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="H15" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" ht="16">
+    <row r="16" spans="1:9" ht="16">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1739,8 +3138,20 @@
       <c r="E16" s="2">
         <v>0.97</v>
       </c>
+      <c r="F16" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" ht="16">
+    <row r="17" spans="1:9" ht="16">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1756,8 +3167,20 @@
       <c r="E17" s="2">
         <v>0.71</v>
       </c>
+      <c r="F17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.59</v>
+      </c>
     </row>
-    <row r="18" spans="1:5" ht="16">
+    <row r="18" spans="1:9" ht="16">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1773,8 +3196,20 @@
       <c r="E18" s="2">
         <v>0.89</v>
       </c>
+      <c r="F18" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" ht="16">
+    <row r="19" spans="1:9" ht="16">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1790,8 +3225,20 @@
       <c r="E19" s="2">
         <v>0.85</v>
       </c>
+      <c r="F19" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.53</v>
+      </c>
     </row>
-    <row r="20" spans="1:5" ht="16">
+    <row r="20" spans="1:9" ht="16">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1807,8 +3254,20 @@
       <c r="E20" s="2">
         <v>0.81</v>
       </c>
+      <c r="F20" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.56999999999999995</v>
+      </c>
     </row>
-    <row r="21" spans="1:5" ht="16">
+    <row r="21" spans="1:9" ht="16">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1824,8 +3283,20 @@
       <c r="E21" s="2">
         <v>0.92</v>
       </c>
+      <c r="F21" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="22" spans="1:5" ht="16">
+    <row r="22" spans="1:9" ht="16">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1841,8 +3312,20 @@
       <c r="E22" s="2">
         <v>0.94</v>
       </c>
+      <c r="F22" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="23" spans="1:5" ht="16">
+    <row r="23" spans="1:9" ht="16">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1858,8 +3341,20 @@
       <c r="E23" s="2">
         <v>1</v>
       </c>
+      <c r="F23" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.49</v>
+      </c>
     </row>
-    <row r="24" spans="1:5" ht="16">
+    <row r="24" spans="1:9" ht="16">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1875,8 +3370,20 @@
       <c r="E24" s="2">
         <v>0.97</v>
       </c>
+      <c r="F24" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.54</v>
+      </c>
     </row>
-    <row r="25" spans="1:5" ht="16">
+    <row r="25" spans="1:9" ht="16">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -1892,8 +3399,20 @@
       <c r="E25" s="2">
         <v>0.84</v>
       </c>
+      <c r="F25" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="26" spans="1:5" ht="16">
+    <row r="26" spans="1:9" ht="16">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -1909,8 +3428,20 @@
       <c r="E26" s="2">
         <v>1</v>
       </c>
+      <c r="F26" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="27" spans="1:5" ht="16">
+    <row r="27" spans="1:9" ht="16">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -1926,8 +3457,20 @@
       <c r="E27" s="2">
         <v>0.82</v>
       </c>
+      <c r="F27" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.73</v>
+      </c>
     </row>
-    <row r="28" spans="1:5" ht="16">
+    <row r="28" spans="1:9" ht="16">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -1943,8 +3486,20 @@
       <c r="E28" s="2">
         <v>0.71</v>
       </c>
+      <c r="F28" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.47</v>
+      </c>
     </row>
-    <row r="29" spans="1:5" ht="16">
+    <row r="29" spans="1:9" ht="16">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -1960,8 +3515,20 @@
       <c r="E29" s="2">
         <v>0.99</v>
       </c>
+      <c r="F29" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.49</v>
+      </c>
     </row>
-    <row r="30" spans="1:5" ht="16">
+    <row r="30" spans="1:9" ht="16">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -1977,8 +3544,20 @@
       <c r="E30" s="2">
         <v>0.97</v>
       </c>
+      <c r="F30" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.48</v>
+      </c>
     </row>
-    <row r="31" spans="1:5" ht="16">
+    <row r="31" spans="1:9" ht="16">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -1994,8 +3573,20 @@
       <c r="E31" s="2">
         <v>0.7</v>
       </c>
+      <c r="F31" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.71</v>
+      </c>
     </row>
-    <row r="32" spans="1:5" ht="16">
+    <row r="32" spans="1:9" ht="16">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -2011,8 +3602,20 @@
       <c r="E32" s="2">
         <v>0.83</v>
       </c>
+      <c r="F32" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.83</v>
+      </c>
     </row>
-    <row r="33" spans="1:5" ht="16">
+    <row r="33" spans="1:9" ht="16">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -2028,8 +3631,20 @@
       <c r="E33" s="2">
         <v>0.79</v>
       </c>
+      <c r="F33" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="34" spans="1:5" ht="16">
+    <row r="34" spans="1:9" ht="16">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -2045,8 +3660,20 @@
       <c r="E34" s="2">
         <v>0.97</v>
       </c>
+      <c r="F34" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.44</v>
+      </c>
     </row>
-    <row r="35" spans="1:5" ht="16">
+    <row r="35" spans="1:9" ht="16">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -2062,8 +3689,20 @@
       <c r="E35" s="2">
         <v>0.96</v>
       </c>
+      <c r="F35" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.68</v>
+      </c>
     </row>
-    <row r="36" spans="1:5" ht="16">
+    <row r="36" spans="1:9" ht="16">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -2079,8 +3718,20 @@
       <c r="E36" s="2">
         <v>0.93</v>
       </c>
+      <c r="F36" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.61</v>
+      </c>
     </row>
-    <row r="37" spans="1:5" ht="16">
+    <row r="37" spans="1:9" ht="16">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -2095,6 +3746,55 @@
       </c>
       <c r="E37" s="2">
         <v>0.94</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <f>AVERAGE(B2:B37)</f>
+        <v>0.1669444444444444</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ref="C39:I39" si="0">AVERAGE(C2:C37)</f>
+        <v>0.13333333333333336</v>
+      </c>
+      <c r="D39">
+        <f>AVERAGE(D2:D37)</f>
+        <v>0.38555555555555565</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0.87944444444444436</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>0.34194444444444438</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>0.53111111111111109</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>7.5833333333333308E-2</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>0.5955555555555555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graph of word speaker performance
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Play</t>
   </si>
@@ -36,19 +36,31 @@
     <t>LogReg word</t>
   </si>
   <si>
-    <t>Naïve Bayes LIWC</t>
-  </si>
-  <si>
     <t>kNN LIWC</t>
   </si>
   <si>
     <t>KMeans LIWC</t>
   </si>
   <si>
-    <t>Decision Tree LIWC</t>
+    <t>Avg</t>
   </si>
   <si>
-    <t>Avg</t>
+    <t>NB word</t>
+  </si>
+  <si>
+    <t>kNN word</t>
+  </si>
+  <si>
+    <t>DT word</t>
+  </si>
+  <si>
+    <t>NB LIWC</t>
+  </si>
+  <si>
+    <t>DT LIWC</t>
+  </si>
+  <si>
+    <t>KMeans word</t>
   </si>
 </sst>
 </file>
@@ -1883,11 +1895,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2069441736"/>
-        <c:axId val="2069444680"/>
+        <c:axId val="2055759448"/>
+        <c:axId val="2055762472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069441736"/>
+        <c:axId val="2055759448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1897,7 +1909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069444680"/>
+        <c:crossAx val="2055762472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1905,7 +1917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069444680"/>
+        <c:axId val="2055762472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1946,7 +1958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2069441736"/>
+        <c:crossAx val="2055759448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2182,11 +2194,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2067920616"/>
-        <c:axId val="2067922888"/>
+        <c:axId val="2055812088"/>
+        <c:axId val="2055815064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2067920616"/>
+        <c:axId val="2055812088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,7 +2208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067922888"/>
+        <c:crossAx val="2055815064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2204,7 +2216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2067922888"/>
+        <c:axId val="2055815064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2245,7 +2257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2067920616"/>
+        <c:crossAx val="2055812088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2283,20 +2295,328 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average classifier speaker prediction performance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>with word features on pruned dataset</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>k Means</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0461111111111111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Decision Tree</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.784444444444444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>kNN</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.248888888888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Naive Bayes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.692777777777777</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Logistic Regression</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.879444444444444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Random</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.166944444444444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Most Common</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.133333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2053153672"/>
+        <c:axId val="2053156648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2053153672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2053156648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2053156648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>F1 Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2053153672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.78260800170249"/>
+          <c:y val="0.229325476472304"/>
+          <c:w val="0.214739625452224"/>
+          <c:h val="0.638042282385935"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2317,16 +2637,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2342,6 +2662,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2672,22 +3024,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16">
+    <row r="1" spans="1:13" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2704,19 +3062,31 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="16">
+    <row r="2" spans="1:13" ht="16">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2744,8 +3114,20 @@
       <c r="I2" s="2">
         <v>0.51</v>
       </c>
+      <c r="J2" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.77</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="16">
+    <row r="3" spans="1:13" ht="16">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2773,8 +3155,20 @@
       <c r="I3" s="2">
         <v>0.63</v>
       </c>
+      <c r="J3" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="16">
+    <row r="4" spans="1:13" ht="16">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2802,8 +3196,20 @@
       <c r="I4" s="2">
         <v>0.55000000000000004</v>
       </c>
+      <c r="J4" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="16">
+    <row r="5" spans="1:13" ht="16">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2831,8 +3237,20 @@
       <c r="I5" s="2">
         <v>0.61</v>
       </c>
+      <c r="J5" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.74</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="16">
+    <row r="6" spans="1:13" ht="16">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2860,8 +3278,20 @@
       <c r="I6" s="2">
         <v>0.63</v>
       </c>
+      <c r="J6" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" ht="16">
+    <row r="7" spans="1:13" ht="16">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2889,8 +3319,20 @@
       <c r="I7" s="2">
         <v>0.47</v>
       </c>
+      <c r="J7" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.78</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="16">
+    <row r="8" spans="1:13" ht="16">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -2918,8 +3360,20 @@
       <c r="I8" s="2">
         <v>0.56000000000000005</v>
       </c>
+      <c r="J8" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.72</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" ht="16">
+    <row r="9" spans="1:13" ht="16">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -2947,8 +3401,20 @@
       <c r="I9" s="2">
         <v>0.77</v>
       </c>
+      <c r="J9" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.85</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" ht="16">
+    <row r="10" spans="1:13" ht="16">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2976,8 +3442,20 @@
       <c r="I10" s="2">
         <v>0.56999999999999995</v>
       </c>
+      <c r="J10" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.83</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" ht="16">
+    <row r="11" spans="1:13" ht="16">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3005,8 +3483,20 @@
       <c r="I11" s="2">
         <v>0.77</v>
       </c>
+      <c r="J11" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.91</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" ht="16">
+    <row r="12" spans="1:13" ht="16">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3034,8 +3524,20 @@
       <c r="I12" s="2">
         <v>0.7</v>
       </c>
+      <c r="J12" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.91</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" ht="16">
+    <row r="13" spans="1:13" ht="16">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3063,8 +3565,20 @@
       <c r="I13" s="2">
         <v>0.55000000000000004</v>
       </c>
+      <c r="J13" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.84</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" ht="16">
+    <row r="14" spans="1:13" ht="16">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3092,8 +3606,20 @@
       <c r="I14" s="2">
         <v>0.57999999999999996</v>
       </c>
+      <c r="J14" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" ht="16">
+    <row r="15" spans="1:13" ht="16">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3121,8 +3647,20 @@
       <c r="I15" s="2">
         <v>0.65</v>
       </c>
+      <c r="J15" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" ht="16">
+    <row r="16" spans="1:13" ht="16">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3150,8 +3688,20 @@
       <c r="I16" s="2">
         <v>0.55000000000000004</v>
       </c>
+      <c r="J16" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.85</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" ht="16">
+    <row r="17" spans="1:13" ht="16">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3179,8 +3729,20 @@
       <c r="I17" s="2">
         <v>0.59</v>
       </c>
+      <c r="J17" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.78</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" ht="16">
+    <row r="18" spans="1:13" ht="16">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3208,8 +3770,20 @@
       <c r="I18" s="2">
         <v>0.4</v>
       </c>
+      <c r="J18" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" ht="16">
+    <row r="19" spans="1:13" ht="16">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3237,8 +3811,20 @@
       <c r="I19" s="2">
         <v>0.53</v>
       </c>
+      <c r="J19" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.73</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" ht="16">
+    <row r="20" spans="1:13" ht="16">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3266,8 +3852,20 @@
       <c r="I20" s="2">
         <v>0.56999999999999995</v>
       </c>
+      <c r="J20" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0.83</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" ht="16">
+    <row r="21" spans="1:13" ht="16">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3295,8 +3893,20 @@
       <c r="I21" s="2">
         <v>0.65</v>
       </c>
+      <c r="J21" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" ht="16">
+    <row r="22" spans="1:13" ht="16">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3324,8 +3934,20 @@
       <c r="I22" s="2">
         <v>0.7</v>
       </c>
+      <c r="J22" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0.71</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" ht="16">
+    <row r="23" spans="1:13" ht="16">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3353,8 +3975,20 @@
       <c r="I23" s="2">
         <v>0.49</v>
       </c>
+      <c r="J23" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" ht="16">
+    <row r="24" spans="1:13" ht="16">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3382,8 +4016,20 @@
       <c r="I24" s="2">
         <v>0.54</v>
       </c>
+      <c r="J24" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.74</v>
+      </c>
     </row>
-    <row r="25" spans="1:9" ht="16">
+    <row r="25" spans="1:13" ht="16">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3411,8 +4057,20 @@
       <c r="I25" s="2">
         <v>0.6</v>
       </c>
+      <c r="J25" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.66</v>
+      </c>
     </row>
-    <row r="26" spans="1:9" ht="16">
+    <row r="26" spans="1:13" ht="16">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3440,8 +4098,20 @@
       <c r="I26" s="2">
         <v>0.65</v>
       </c>
+      <c r="J26" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0.82</v>
+      </c>
     </row>
-    <row r="27" spans="1:9" ht="16">
+    <row r="27" spans="1:13" ht="16">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3469,8 +4139,20 @@
       <c r="I27" s="2">
         <v>0.73</v>
       </c>
+      <c r="J27" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0.89</v>
+      </c>
     </row>
-    <row r="28" spans="1:9" ht="16">
+    <row r="28" spans="1:13" ht="16">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3498,8 +4180,20 @@
       <c r="I28" s="2">
         <v>0.47</v>
       </c>
+      <c r="J28" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="29" spans="1:9" ht="16">
+    <row r="29" spans="1:13" ht="16">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -3527,8 +4221,20 @@
       <c r="I29" s="2">
         <v>0.49</v>
       </c>
+      <c r="J29" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0.77</v>
+      </c>
     </row>
-    <row r="30" spans="1:9" ht="16">
+    <row r="30" spans="1:13" ht="16">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -3556,8 +4262,20 @@
       <c r="I30" s="2">
         <v>0.48</v>
       </c>
+      <c r="J30" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0.79</v>
+      </c>
     </row>
-    <row r="31" spans="1:9" ht="16">
+    <row r="31" spans="1:13" ht="16">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -3585,8 +4303,20 @@
       <c r="I31" s="2">
         <v>0.71</v>
       </c>
+      <c r="J31" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.85</v>
+      </c>
     </row>
-    <row r="32" spans="1:9" ht="16">
+    <row r="32" spans="1:13" ht="16">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -3614,8 +4344,20 @@
       <c r="I32" s="2">
         <v>0.83</v>
       </c>
+      <c r="J32" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0.82</v>
+      </c>
     </row>
-    <row r="33" spans="1:9" ht="16">
+    <row r="33" spans="1:13" ht="16">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -3643,8 +4385,20 @@
       <c r="I33" s="2">
         <v>0.7</v>
       </c>
+      <c r="J33" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.71</v>
+      </c>
     </row>
-    <row r="34" spans="1:9" ht="16">
+    <row r="34" spans="1:13" ht="16">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -3672,8 +4426,20 @@
       <c r="I34" s="2">
         <v>0.44</v>
       </c>
+      <c r="J34" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0.71</v>
+      </c>
     </row>
-    <row r="35" spans="1:9" ht="16">
+    <row r="35" spans="1:13" ht="16">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -3701,8 +4467,20 @@
       <c r="I35" s="2">
         <v>0.68</v>
       </c>
+      <c r="J35" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="K35" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L35" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0.68</v>
+      </c>
     </row>
-    <row r="36" spans="1:9" ht="16">
+    <row r="36" spans="1:13" ht="16">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -3730,8 +4508,20 @@
       <c r="I36" s="2">
         <v>0.61</v>
       </c>
+      <c r="J36" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="37" spans="1:9" ht="16">
+    <row r="37" spans="1:13" ht="16">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -3759,17 +4549,29 @@
       <c r="I37" s="2">
         <v>0.48</v>
       </c>
+      <c r="J37" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0.74</v>
+      </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39">
         <f>AVERAGE(B2:B37)</f>
         <v>0.1669444444444444</v>
       </c>
       <c r="C39">
-        <f t="shared" ref="C39:I39" si="0">AVERAGE(C2:C37)</f>
+        <f t="shared" ref="C39:M39" si="0">AVERAGE(C2:C37)</f>
         <v>0.13333333333333336</v>
       </c>
       <c r="D39">
@@ -3795,6 +4597,22 @@
       <c r="I39">
         <f t="shared" si="0"/>
         <v>0.5955555555555555</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>0.6927777777777776</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>0.24888888888888891</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>4.6111111111111124E-2</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>0.78444444444444439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started making listener graphs.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Play</t>
   </si>
@@ -62,12 +62,18 @@
   <si>
     <t>KMeans word</t>
   </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +91,30 @@
       <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,15 +134,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="21">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1895,11 +1966,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2055759448"/>
-        <c:axId val="2055762472"/>
+        <c:axId val="2097051352"/>
+        <c:axId val="2097054328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2055759448"/>
+        <c:axId val="2097051352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2055762472"/>
+        <c:crossAx val="2097054328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1917,7 +1988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2055762472"/>
+        <c:axId val="2097054328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1958,7 +2029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2055759448"/>
+        <c:crossAx val="2097051352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2194,11 +2265,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2055812088"/>
-        <c:axId val="2055815064"/>
+        <c:axId val="2096496440"/>
+        <c:axId val="2096493448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2055812088"/>
+        <c:axId val="2096496440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2279,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2055815064"/>
+        <c:crossAx val="2096493448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2216,7 +2287,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2055815064"/>
+        <c:axId val="2096493448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2257,7 +2328,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2055812088"/>
+        <c:crossAx val="2096496440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2493,11 +2564,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2053153672"/>
-        <c:axId val="2053156648"/>
+        <c:axId val="2096449176"/>
+        <c:axId val="2096446184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2053153672"/>
+        <c:axId val="2096449176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2507,7 +2578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2053156648"/>
+        <c:crossAx val="2096446184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2515,7 +2586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2053156648"/>
+        <c:axId val="2096446184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2556,7 +2627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2053153672"/>
+        <c:crossAx val="2096449176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3024,25 +3095,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:AE150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" customWidth="1"/>
+    <col min="2" max="3" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="7" width="5.1640625" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" customWidth="1"/>
+    <col min="11" max="11" width="5.5" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="13" width="5.5" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" customWidth="1"/>
+    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" customWidth="1"/>
+    <col min="17" max="17" width="5.33203125" customWidth="1"/>
+    <col min="18" max="18" width="5.1640625" customWidth="1"/>
+    <col min="19" max="20" width="4.83203125" customWidth="1"/>
+    <col min="21" max="22" width="5.1640625" customWidth="1"/>
+    <col min="23" max="23" width="5" customWidth="1"/>
+    <col min="24" max="24" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5" customWidth="1"/>
+    <col min="26" max="26" width="4.83203125" customWidth="1"/>
+    <col min="27" max="27" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5" customWidth="1"/>
+    <col min="29" max="29" width="5.1640625" customWidth="1"/>
+    <col min="30" max="30" width="8.33203125" customWidth="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
+    <col min="32" max="32" width="7.33203125" customWidth="1"/>
+    <col min="33" max="33" width="5" customWidth="1"/>
+    <col min="34" max="34" width="5.6640625" customWidth="1"/>
+    <col min="35" max="36" width="4.83203125" customWidth="1"/>
+    <col min="37" max="37" width="5" customWidth="1"/>
+    <col min="38" max="38" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16">
@@ -4357,7 +4450,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16">
+    <row r="33" spans="1:31" ht="16">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -4398,7 +4491,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="16">
+    <row r="34" spans="1:31" ht="16">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -4439,7 +4532,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16">
+    <row r="35" spans="1:31" ht="16">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -4480,7 +4573,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16">
+    <row r="36" spans="1:31" ht="16">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -4521,7 +4614,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="16">
+    <row r="37" spans="1:31" ht="16">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -4562,7 +4655,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4615,8 +4708,2309 @@
         <v>0.78444444444444439</v>
       </c>
     </row>
+    <row r="44" spans="1:31">
+      <c r="A44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE44" s="3"/>
+    </row>
+    <row r="45" spans="1:31">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>0.06</v>
+      </c>
+      <c r="C45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.03</v>
+      </c>
+      <c r="F45">
+        <v>0.05</v>
+      </c>
+      <c r="G45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H45">
+        <v>0.04</v>
+      </c>
+      <c r="I45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J45">
+        <v>0.09</v>
+      </c>
+      <c r="K45">
+        <v>0.05</v>
+      </c>
+      <c r="L45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M45">
+        <v>0.1</v>
+      </c>
+      <c r="N45">
+        <v>0.06</v>
+      </c>
+      <c r="AD45">
+        <f>AVERAGE(B45:N45)</f>
+        <v>5.8461538461538461E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31">
+      <c r="A48">
+        <f>A45+1</f>
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>0.01</v>
+      </c>
+      <c r="C48">
+        <v>0.04</v>
+      </c>
+      <c r="D48">
+        <v>0.03</v>
+      </c>
+      <c r="E48">
+        <v>0.04</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0.02</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0.03</v>
+      </c>
+      <c r="L48">
+        <v>0.02</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0.01</v>
+      </c>
+      <c r="P48">
+        <v>0.02</v>
+      </c>
+      <c r="Q48">
+        <v>0.05</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0.03</v>
+      </c>
+      <c r="T48">
+        <v>0.03</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <v>0.05</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>0.02</v>
+      </c>
+      <c r="Z48">
+        <v>0.06</v>
+      </c>
+      <c r="AD48">
+        <f>AVERAGE(B48:Z48)</f>
+        <v>1.84E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30">
+      <c r="A51">
+        <f>A48+1</f>
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>0.06</v>
+      </c>
+      <c r="C51">
+        <v>0.05</v>
+      </c>
+      <c r="D51">
+        <v>0.06</v>
+      </c>
+      <c r="E51">
+        <v>0.05</v>
+      </c>
+      <c r="F51">
+        <v>0.05</v>
+      </c>
+      <c r="G51">
+        <v>0.04</v>
+      </c>
+      <c r="H51">
+        <v>0.11</v>
+      </c>
+      <c r="I51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J51">
+        <v>0.04</v>
+      </c>
+      <c r="K51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L51">
+        <v>0.06</v>
+      </c>
+      <c r="M51">
+        <v>0.04</v>
+      </c>
+      <c r="N51">
+        <v>0.09</v>
+      </c>
+      <c r="O51">
+        <v>0.16</v>
+      </c>
+      <c r="AD51">
+        <f>AVERAGE(B51:O51)</f>
+        <v>6.7857142857142852E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30">
+      <c r="A54">
+        <f>A51+1</f>
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>0.02</v>
+      </c>
+      <c r="C54">
+        <v>0.13</v>
+      </c>
+      <c r="D54">
+        <v>0.08</v>
+      </c>
+      <c r="E54">
+        <v>0.06</v>
+      </c>
+      <c r="F54">
+        <v>0.06</v>
+      </c>
+      <c r="G54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H54">
+        <v>0.04</v>
+      </c>
+      <c r="I54">
+        <v>0.04</v>
+      </c>
+      <c r="J54">
+        <v>0.05</v>
+      </c>
+      <c r="K54">
+        <v>0.08</v>
+      </c>
+      <c r="L54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M54">
+        <v>0.04</v>
+      </c>
+      <c r="N54">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O54">
+        <v>0.06</v>
+      </c>
+      <c r="AD54">
+        <f>AVERAGE(B54:O54)</f>
+        <v>6.7142857142857143E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30">
+      <c r="A57">
+        <f>A54+1</f>
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0.02</v>
+      </c>
+      <c r="D57">
+        <v>0.03</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0.01</v>
+      </c>
+      <c r="G57">
+        <v>0.03</v>
+      </c>
+      <c r="H57">
+        <v>0.02</v>
+      </c>
+      <c r="I57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J57">
+        <v>0.02</v>
+      </c>
+      <c r="K57">
+        <v>0.05</v>
+      </c>
+      <c r="L57">
+        <v>0.02</v>
+      </c>
+      <c r="M57">
+        <v>0.06</v>
+      </c>
+      <c r="N57">
+        <v>0.03</v>
+      </c>
+      <c r="O57">
+        <v>0.02</v>
+      </c>
+      <c r="P57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q57">
+        <v>0.02</v>
+      </c>
+      <c r="R57">
+        <v>0.03</v>
+      </c>
+      <c r="S57">
+        <v>0.05</v>
+      </c>
+      <c r="T57">
+        <v>0</v>
+      </c>
+      <c r="U57">
+        <v>0</v>
+      </c>
+      <c r="V57">
+        <v>0.06</v>
+      </c>
+      <c r="AD57">
+        <f>AVERAGE(B57:V57)</f>
+        <v>2.9047619047619051E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30">
+      <c r="A60">
+        <f>A57+1</f>
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C60">
+        <v>0.04</v>
+      </c>
+      <c r="D60">
+        <v>0.02</v>
+      </c>
+      <c r="E60">
+        <v>0.06</v>
+      </c>
+      <c r="F60">
+        <v>0.04</v>
+      </c>
+      <c r="G60">
+        <v>0.03</v>
+      </c>
+      <c r="H60">
+        <v>0.03</v>
+      </c>
+      <c r="I60">
+        <v>0.03</v>
+      </c>
+      <c r="J60">
+        <v>0.04</v>
+      </c>
+      <c r="K60">
+        <v>0.08</v>
+      </c>
+      <c r="L60">
+        <v>0.04</v>
+      </c>
+      <c r="M60">
+        <v>0.09</v>
+      </c>
+      <c r="N60">
+        <v>0.05</v>
+      </c>
+      <c r="O60">
+        <v>0.02</v>
+      </c>
+      <c r="P60">
+        <v>0.01</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>0.1</v>
+      </c>
+      <c r="S60">
+        <v>0.13</v>
+      </c>
+      <c r="AD60">
+        <f>AVERAGE(B60:S60)</f>
+        <v>4.8888888888888898E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30">
+      <c r="A63">
+        <f>A60+1</f>
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>0.02</v>
+      </c>
+      <c r="C63">
+        <v>0.11</v>
+      </c>
+      <c r="D63">
+        <v>0.02</v>
+      </c>
+      <c r="E63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0.02</v>
+      </c>
+      <c r="H63">
+        <v>0.08</v>
+      </c>
+      <c r="I63">
+        <v>0.03</v>
+      </c>
+      <c r="J63">
+        <v>0.03</v>
+      </c>
+      <c r="K63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L63">
+        <v>0.03</v>
+      </c>
+      <c r="M63">
+        <v>0.03</v>
+      </c>
+      <c r="N63">
+        <v>0.03</v>
+      </c>
+      <c r="O63">
+        <v>0.15</v>
+      </c>
+      <c r="P63">
+        <v>0.04</v>
+      </c>
+      <c r="Q63">
+        <v>0.02</v>
+      </c>
+      <c r="R63">
+        <v>0.04</v>
+      </c>
+      <c r="S63">
+        <v>0.06</v>
+      </c>
+      <c r="AD63">
+        <f>AVERAGE(B63:S63)</f>
+        <v>4.7222222222222228E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30">
+      <c r="A66">
+        <f>A63+1</f>
+        <v>7</v>
+      </c>
+      <c r="B66">
+        <v>0.08</v>
+      </c>
+      <c r="C66">
+        <v>0.15</v>
+      </c>
+      <c r="D66">
+        <v>0.02</v>
+      </c>
+      <c r="E66">
+        <v>0.05</v>
+      </c>
+      <c r="F66">
+        <v>0.03</v>
+      </c>
+      <c r="G66">
+        <v>0.11</v>
+      </c>
+      <c r="H66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I66">
+        <v>0.03</v>
+      </c>
+      <c r="J66">
+        <v>0.02</v>
+      </c>
+      <c r="K66">
+        <v>0.06</v>
+      </c>
+      <c r="L66">
+        <v>0.03</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0.05</v>
+      </c>
+      <c r="O66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q66">
+        <v>0.05</v>
+      </c>
+      <c r="R66">
+        <v>0.03</v>
+      </c>
+      <c r="S66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AD66">
+        <f>AVERAGE(B66:S66)</f>
+        <v>5.5000000000000021E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30">
+      <c r="A69">
+        <f>A66+1</f>
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>0.03</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0.03</v>
+      </c>
+      <c r="E69">
+        <v>0.04</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0.02</v>
+      </c>
+      <c r="H69">
+        <v>0.03</v>
+      </c>
+      <c r="I69">
+        <v>0.03</v>
+      </c>
+      <c r="J69">
+        <v>0.03</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0.04</v>
+      </c>
+      <c r="M69">
+        <v>0.04</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0.09</v>
+      </c>
+      <c r="S69">
+        <v>0.05</v>
+      </c>
+      <c r="T69">
+        <v>0.04</v>
+      </c>
+      <c r="U69">
+        <v>0.03</v>
+      </c>
+      <c r="V69">
+        <v>0.02</v>
+      </c>
+      <c r="W69">
+        <v>0.01</v>
+      </c>
+      <c r="X69">
+        <v>0.04</v>
+      </c>
+      <c r="Y69">
+        <v>0.02</v>
+      </c>
+      <c r="Z69">
+        <v>0</v>
+      </c>
+      <c r="AA69">
+        <v>0.05</v>
+      </c>
+      <c r="AB69">
+        <v>0</v>
+      </c>
+      <c r="AD69">
+        <f>AVERAGE(B69:AB69)</f>
+        <v>2.3703703703703709E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30">
+      <c r="A72">
+        <f>A69+1</f>
+        <v>9</v>
+      </c>
+      <c r="B72">
+        <v>0.09</v>
+      </c>
+      <c r="C72">
+        <v>0.11</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0.03</v>
+      </c>
+      <c r="I72">
+        <v>0.04</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0.05</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0.02</v>
+      </c>
+      <c r="P72">
+        <v>0.04</v>
+      </c>
+      <c r="Q72">
+        <v>0.02</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0.03</v>
+      </c>
+      <c r="T72">
+        <v>0.05</v>
+      </c>
+      <c r="U72">
+        <v>0</v>
+      </c>
+      <c r="V72">
+        <v>0.1</v>
+      </c>
+      <c r="W72">
+        <v>0</v>
+      </c>
+      <c r="X72">
+        <v>0.04</v>
+      </c>
+      <c r="Y72">
+        <v>0.04</v>
+      </c>
+      <c r="Z72">
+        <v>0.02</v>
+      </c>
+      <c r="AD72">
+        <f>AVERAGE(B72:Z72)</f>
+        <v>3.0000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30">
+      <c r="A75">
+        <f>A72+1</f>
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0.06</v>
+      </c>
+      <c r="D75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E75">
+        <v>0.02</v>
+      </c>
+      <c r="F75">
+        <v>0.05</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0.02</v>
+      </c>
+      <c r="I75">
+        <v>0.06</v>
+      </c>
+      <c r="J75">
+        <v>0.02</v>
+      </c>
+      <c r="K75">
+        <v>0.04</v>
+      </c>
+      <c r="L75">
+        <v>0.01</v>
+      </c>
+      <c r="M75">
+        <v>0.04</v>
+      </c>
+      <c r="N75">
+        <v>0.03</v>
+      </c>
+      <c r="O75">
+        <v>0.05</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0.03</v>
+      </c>
+      <c r="R75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S75">
+        <v>0.04</v>
+      </c>
+      <c r="T75">
+        <v>0.05</v>
+      </c>
+      <c r="U75">
+        <v>0.03</v>
+      </c>
+      <c r="V75">
+        <v>0.05</v>
+      </c>
+      <c r="AD75">
+        <f>AVERAGE(B75:V75)</f>
+        <v>3.5238095238095249E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30">
+      <c r="A78">
+        <f>A75+1</f>
+        <v>11</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0.02</v>
+      </c>
+      <c r="E78">
+        <v>0.02</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0.08</v>
+      </c>
+      <c r="H78">
+        <v>0.06</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0.04</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0.09</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0.02</v>
+      </c>
+      <c r="R78">
+        <v>0.02</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78">
+        <v>0.03</v>
+      </c>
+      <c r="U78">
+        <v>0</v>
+      </c>
+      <c r="V78">
+        <v>0.04</v>
+      </c>
+      <c r="W78">
+        <v>0.03</v>
+      </c>
+      <c r="X78">
+        <v>0.02</v>
+      </c>
+      <c r="Y78">
+        <v>0.05</v>
+      </c>
+      <c r="Z78">
+        <v>0.02</v>
+      </c>
+      <c r="AA78">
+        <v>0.02</v>
+      </c>
+      <c r="AD78">
+        <f>AVERAGE(B78:AA78)</f>
+        <v>2.1538461538461541E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30">
+      <c r="A81">
+        <f>A78+1</f>
+        <v>12</v>
+      </c>
+      <c r="B81">
+        <v>0.02</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0.06</v>
+      </c>
+      <c r="E81">
+        <v>0.03</v>
+      </c>
+      <c r="F81">
+        <v>0.08</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0.03</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0.03</v>
+      </c>
+      <c r="K81">
+        <v>0.03</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0.06</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
+      <c r="P81">
+        <v>0.03</v>
+      </c>
+      <c r="Q81">
+        <v>0.04</v>
+      </c>
+      <c r="R81">
+        <v>0.03</v>
+      </c>
+      <c r="S81">
+        <v>0.02</v>
+      </c>
+      <c r="T81">
+        <v>0.02</v>
+      </c>
+      <c r="AD81">
+        <f>AVERAGE(B81:T81)</f>
+        <v>2.5263157894736842E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30">
+      <c r="A84">
+        <f>A81+1</f>
+        <v>13</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0.02</v>
+      </c>
+      <c r="D84">
+        <v>0.04</v>
+      </c>
+      <c r="E84">
+        <v>0.04</v>
+      </c>
+      <c r="F84">
+        <v>0.04</v>
+      </c>
+      <c r="G84">
+        <v>0.02</v>
+      </c>
+      <c r="H84">
+        <v>0.04</v>
+      </c>
+      <c r="I84">
+        <v>0.16</v>
+      </c>
+      <c r="J84">
+        <v>0.03</v>
+      </c>
+      <c r="K84">
+        <v>0.03</v>
+      </c>
+      <c r="L84">
+        <v>0.06</v>
+      </c>
+      <c r="M84">
+        <v>0.03</v>
+      </c>
+      <c r="N84">
+        <v>0.06</v>
+      </c>
+      <c r="O84">
+        <v>0.06</v>
+      </c>
+      <c r="P84">
+        <v>0.03</v>
+      </c>
+      <c r="Q84">
+        <v>0.04</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+      <c r="S84">
+        <v>0.06</v>
+      </c>
+      <c r="T84">
+        <v>0.05</v>
+      </c>
+      <c r="U84">
+        <v>0.02</v>
+      </c>
+      <c r="V84">
+        <v>0.09</v>
+      </c>
+      <c r="AD84">
+        <f>AVERAGE(B84:V84)</f>
+        <v>4.3809523809523819E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:30">
+      <c r="A87">
+        <f>A84+1</f>
+        <v>14</v>
+      </c>
+      <c r="B87">
+        <v>0.04</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0.06</v>
+      </c>
+      <c r="E87">
+        <v>0.05</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0.02</v>
+      </c>
+      <c r="I87">
+        <v>0.05</v>
+      </c>
+      <c r="J87">
+        <v>0.05</v>
+      </c>
+      <c r="K87">
+        <v>0.05</v>
+      </c>
+      <c r="L87">
+        <v>0.1</v>
+      </c>
+      <c r="M87">
+        <v>0.17</v>
+      </c>
+      <c r="N87">
+        <v>0.06</v>
+      </c>
+      <c r="O87">
+        <v>0.06</v>
+      </c>
+      <c r="P87">
+        <v>0.03</v>
+      </c>
+      <c r="Q87">
+        <v>0.03</v>
+      </c>
+      <c r="R87">
+        <v>0.04</v>
+      </c>
+      <c r="AD87">
+        <f>AVERAGE(B87:R87)</f>
+        <v>4.7647058823529431E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:30">
+      <c r="A90">
+        <f>A87+1</f>
+        <v>15</v>
+      </c>
+      <c r="B90">
+        <v>0.05</v>
+      </c>
+      <c r="C90">
+        <v>0.06</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0.03</v>
+      </c>
+      <c r="F90">
+        <v>0.02</v>
+      </c>
+      <c r="G90">
+        <v>0.03</v>
+      </c>
+      <c r="H90">
+        <v>0.04</v>
+      </c>
+      <c r="I90">
+        <v>0.03</v>
+      </c>
+      <c r="J90">
+        <v>0.12</v>
+      </c>
+      <c r="K90">
+        <v>0.02</v>
+      </c>
+      <c r="L90">
+        <v>0.03</v>
+      </c>
+      <c r="M90">
+        <v>0.04</v>
+      </c>
+      <c r="N90">
+        <v>0.03</v>
+      </c>
+      <c r="O90">
+        <v>0.03</v>
+      </c>
+      <c r="P90">
+        <v>0.04</v>
+      </c>
+      <c r="Q90">
+        <v>0.02</v>
+      </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+      <c r="S90">
+        <v>0.02</v>
+      </c>
+      <c r="T90">
+        <v>0.06</v>
+      </c>
+      <c r="U90">
+        <v>0.05</v>
+      </c>
+      <c r="V90">
+        <v>0.05</v>
+      </c>
+      <c r="AD90">
+        <f>AVERAGE(B90:V90)</f>
+        <v>3.6666666666666681E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:30">
+      <c r="A93">
+        <f>A90+1</f>
+        <v>16</v>
+      </c>
+      <c r="B93">
+        <v>0.06</v>
+      </c>
+      <c r="C93">
+        <v>0.05</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0.06</v>
+      </c>
+      <c r="F93">
+        <v>0.04</v>
+      </c>
+      <c r="G93">
+        <v>0.09</v>
+      </c>
+      <c r="H93">
+        <v>0.08</v>
+      </c>
+      <c r="I93">
+        <v>0.08</v>
+      </c>
+      <c r="J93">
+        <v>0.04</v>
+      </c>
+      <c r="K93">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L93">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M93">
+        <v>0.03</v>
+      </c>
+      <c r="N93">
+        <v>0.08</v>
+      </c>
+      <c r="O93">
+        <v>0.05</v>
+      </c>
+      <c r="P93">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q93">
+        <v>0.05</v>
+      </c>
+      <c r="AD93">
+        <f>AVERAGE(B93:Q93)</f>
+        <v>5.7500000000000009E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:30">
+      <c r="A96">
+        <f>A93+1</f>
+        <v>17</v>
+      </c>
+      <c r="B96">
+        <v>0.06</v>
+      </c>
+      <c r="C96">
+        <v>0.08</v>
+      </c>
+      <c r="D96">
+        <v>0.02</v>
+      </c>
+      <c r="E96">
+        <v>0.06</v>
+      </c>
+      <c r="F96">
+        <v>0.03</v>
+      </c>
+      <c r="G96">
+        <v>0.06</v>
+      </c>
+      <c r="H96">
+        <v>0.09</v>
+      </c>
+      <c r="I96">
+        <v>0.05</v>
+      </c>
+      <c r="J96">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K96">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L96">
+        <v>0.05</v>
+      </c>
+      <c r="M96">
+        <v>0.06</v>
+      </c>
+      <c r="N96">
+        <v>0.06</v>
+      </c>
+      <c r="O96">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P96">
+        <v>0.06</v>
+      </c>
+      <c r="Q96">
+        <v>0.06</v>
+      </c>
+      <c r="AD96">
+        <f>AVERAGE(B96:Q96)</f>
+        <v>5.9375000000000025E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:30">
+      <c r="A99">
+        <f>A96+1</f>
+        <v>18</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0.03</v>
+      </c>
+      <c r="D99">
+        <v>0.04</v>
+      </c>
+      <c r="E99">
+        <v>0.15</v>
+      </c>
+      <c r="F99">
+        <v>0.09</v>
+      </c>
+      <c r="G99">
+        <v>0.02</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0.05</v>
+      </c>
+      <c r="J99">
+        <v>0.09</v>
+      </c>
+      <c r="K99">
+        <v>0.04</v>
+      </c>
+      <c r="L99">
+        <v>0.03</v>
+      </c>
+      <c r="M99">
+        <v>0.03</v>
+      </c>
+      <c r="N99">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0.08</v>
+      </c>
+      <c r="AD99">
+        <f>AVERAGE(B99:Q99)</f>
+        <v>5.2666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30">
+      <c r="A102">
+        <f>A99+1</f>
+        <v>19</v>
+      </c>
+      <c r="B102">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C102">
+        <v>0.16</v>
+      </c>
+      <c r="D102">
+        <v>0.03</v>
+      </c>
+      <c r="E102">
+        <v>0.09</v>
+      </c>
+      <c r="F102">
+        <v>0.12</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0.05</v>
+      </c>
+      <c r="I102">
+        <v>0.11</v>
+      </c>
+      <c r="J102">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K102">
+        <v>0.05</v>
+      </c>
+      <c r="L102">
+        <v>0.05</v>
+      </c>
+      <c r="M102">
+        <v>0.02</v>
+      </c>
+      <c r="N102">
+        <v>0.05</v>
+      </c>
+      <c r="O102">
+        <v>0.05</v>
+      </c>
+      <c r="AD102">
+        <f>AVERAGE(B102:O102)</f>
+        <v>6.5714285714285725E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:30">
+      <c r="A105">
+        <f>A102+1</f>
+        <v>20</v>
+      </c>
+      <c r="B105">
+        <v>0.06</v>
+      </c>
+      <c r="C105">
+        <v>0.04</v>
+      </c>
+      <c r="D105">
+        <v>0.05</v>
+      </c>
+      <c r="E105">
+        <v>0.04</v>
+      </c>
+      <c r="F105">
+        <v>0.05</v>
+      </c>
+      <c r="G105">
+        <v>0.03</v>
+      </c>
+      <c r="H105">
+        <v>0.06</v>
+      </c>
+      <c r="I105">
+        <v>0.04</v>
+      </c>
+      <c r="J105">
+        <v>0.04</v>
+      </c>
+      <c r="K105">
+        <v>0.06</v>
+      </c>
+      <c r="L105">
+        <v>0.08</v>
+      </c>
+      <c r="M105">
+        <v>0.05</v>
+      </c>
+      <c r="N105">
+        <v>0.05</v>
+      </c>
+      <c r="O105">
+        <v>0.04</v>
+      </c>
+      <c r="P105">
+        <v>0.06</v>
+      </c>
+      <c r="Q105">
+        <v>0.06</v>
+      </c>
+      <c r="R105">
+        <v>0.05</v>
+      </c>
+      <c r="AD105">
+        <f>AVERAGE(B105:R105)</f>
+        <v>5.0588235294117656E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30">
+      <c r="A108">
+        <f>A105+1</f>
+        <v>21</v>
+      </c>
+      <c r="B108">
+        <v>0.05</v>
+      </c>
+      <c r="C108">
+        <v>0.04</v>
+      </c>
+      <c r="D108">
+        <v>0.05</v>
+      </c>
+      <c r="E108">
+        <v>0.06</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H108">
+        <v>0.03</v>
+      </c>
+      <c r="I108">
+        <v>0.04</v>
+      </c>
+      <c r="J108">
+        <v>0.04</v>
+      </c>
+      <c r="K108">
+        <v>0.01</v>
+      </c>
+      <c r="L108">
+        <v>0.08</v>
+      </c>
+      <c r="M108">
+        <v>0.05</v>
+      </c>
+      <c r="N108">
+        <v>0.09</v>
+      </c>
+      <c r="O108">
+        <v>0.04</v>
+      </c>
+      <c r="P108">
+        <v>0.05</v>
+      </c>
+      <c r="Q108">
+        <v>0</v>
+      </c>
+      <c r="R108">
+        <v>0.08</v>
+      </c>
+      <c r="AD108">
+        <f>AVERAGE(B108:R108)</f>
+        <v>4.5882352941176471E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:30">
+      <c r="A111">
+        <f>A108+1</f>
+        <v>22</v>
+      </c>
+      <c r="B111">
+        <v>0.06</v>
+      </c>
+      <c r="C111">
+        <v>0.12</v>
+      </c>
+      <c r="D111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F111">
+        <v>0.04</v>
+      </c>
+      <c r="G111">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H111">
+        <v>0.06</v>
+      </c>
+      <c r="I111">
+        <v>0.04</v>
+      </c>
+      <c r="J111">
+        <v>0.04</v>
+      </c>
+      <c r="K111">
+        <v>0.08</v>
+      </c>
+      <c r="L111">
+        <v>0.06</v>
+      </c>
+      <c r="M111">
+        <v>0.03</v>
+      </c>
+      <c r="N111">
+        <v>0.08</v>
+      </c>
+      <c r="O111">
+        <v>0.06</v>
+      </c>
+      <c r="P111">
+        <v>0.08</v>
+      </c>
+      <c r="Q111">
+        <v>0.05</v>
+      </c>
+      <c r="R111">
+        <v>0.06</v>
+      </c>
+      <c r="S111">
+        <v>0.04</v>
+      </c>
+      <c r="T111">
+        <v>0.06</v>
+      </c>
+      <c r="AD111">
+        <f>AVERAGE(B111:T111)</f>
+        <v>6.1578947368421046E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:30">
+      <c r="A114">
+        <f>A111+1</f>
+        <v>23</v>
+      </c>
+      <c r="B114">
+        <v>0.04</v>
+      </c>
+      <c r="C114">
+        <v>0.04</v>
+      </c>
+      <c r="D114">
+        <v>0.06</v>
+      </c>
+      <c r="E114">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F114">
+        <v>0.1</v>
+      </c>
+      <c r="G114">
+        <v>0.04</v>
+      </c>
+      <c r="H114">
+        <v>0.04</v>
+      </c>
+      <c r="I114">
+        <v>0.09</v>
+      </c>
+      <c r="J114">
+        <v>0.03</v>
+      </c>
+      <c r="K114">
+        <v>0.02</v>
+      </c>
+      <c r="L114">
+        <v>0.05</v>
+      </c>
+      <c r="M114">
+        <v>0.04</v>
+      </c>
+      <c r="N114">
+        <v>0.05</v>
+      </c>
+      <c r="O114">
+        <v>0.09</v>
+      </c>
+      <c r="P114">
+        <v>0.06</v>
+      </c>
+      <c r="AD114">
+        <f>AVERAGE(B114:P114)</f>
+        <v>5.4666666666666669E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:30">
+      <c r="A117">
+        <f>A114+1</f>
+        <v>24</v>
+      </c>
+      <c r="B117">
+        <v>0.04</v>
+      </c>
+      <c r="C117">
+        <v>0.06</v>
+      </c>
+      <c r="D117">
+        <v>0.04</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <v>0.02</v>
+      </c>
+      <c r="H117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I117">
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <v>0.04</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>0.06</v>
+      </c>
+      <c r="M117">
+        <v>0</v>
+      </c>
+      <c r="N117">
+        <v>0.02</v>
+      </c>
+      <c r="O117">
+        <v>0.11</v>
+      </c>
+      <c r="P117">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q117">
+        <v>0.03</v>
+      </c>
+      <c r="AD117">
+        <f>AVERAGE(B117:Q117)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:30">
+      <c r="A120">
+        <f>A117+1</f>
+        <v>25</v>
+      </c>
+      <c r="B120">
+        <v>0.03</v>
+      </c>
+      <c r="C120">
+        <v>0.02</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0.02</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>0.05</v>
+      </c>
+      <c r="H120">
+        <v>0.05</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0.02</v>
+      </c>
+      <c r="L120">
+        <v>0.02</v>
+      </c>
+      <c r="M120">
+        <v>0</v>
+      </c>
+      <c r="N120">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O120">
+        <v>0.02</v>
+      </c>
+      <c r="P120">
+        <v>0.05</v>
+      </c>
+      <c r="Q120">
+        <v>0.02</v>
+      </c>
+      <c r="R120">
+        <v>0.05</v>
+      </c>
+      <c r="S120">
+        <v>0.03</v>
+      </c>
+      <c r="T120">
+        <v>0.01</v>
+      </c>
+      <c r="U120">
+        <v>0.06</v>
+      </c>
+      <c r="V120">
+        <v>0.02</v>
+      </c>
+      <c r="AD120">
+        <f>AVERAGE(B120:V120)</f>
+        <v>2.5714285714285717E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:30">
+      <c r="A123">
+        <f>A120+1</f>
+        <v>26</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0.05</v>
+      </c>
+      <c r="D123">
+        <v>0.05</v>
+      </c>
+      <c r="E123">
+        <v>0.03</v>
+      </c>
+      <c r="F123">
+        <v>0.03</v>
+      </c>
+      <c r="G123">
+        <v>0.05</v>
+      </c>
+      <c r="H123">
+        <v>0.04</v>
+      </c>
+      <c r="I123">
+        <v>0.02</v>
+      </c>
+      <c r="J123">
+        <v>0.05</v>
+      </c>
+      <c r="K123">
+        <v>0.02</v>
+      </c>
+      <c r="L123">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M123">
+        <v>0.13</v>
+      </c>
+      <c r="N123">
+        <v>0.02</v>
+      </c>
+      <c r="O123">
+        <v>0.05</v>
+      </c>
+      <c r="P123">
+        <v>0.05</v>
+      </c>
+      <c r="Q123">
+        <v>0.1</v>
+      </c>
+      <c r="R123">
+        <v>0</v>
+      </c>
+      <c r="S123">
+        <v>0.19</v>
+      </c>
+      <c r="T123">
+        <v>0.05</v>
+      </c>
+      <c r="AD123">
+        <f>AVERAGE(B123:T123)</f>
+        <v>5.2631578947368432E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30">
+      <c r="A126">
+        <f>A123+1</f>
+        <v>27</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>0.04</v>
+      </c>
+      <c r="D126">
+        <v>0.03</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>0.03</v>
+      </c>
+      <c r="G126">
+        <v>0.05</v>
+      </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
+      <c r="I126">
+        <v>0.09</v>
+      </c>
+      <c r="J126">
+        <v>0.02</v>
+      </c>
+      <c r="K126">
+        <v>0.03</v>
+      </c>
+      <c r="L126">
+        <v>0.03</v>
+      </c>
+      <c r="M126">
+        <v>0.09</v>
+      </c>
+      <c r="N126">
+        <v>0.03</v>
+      </c>
+      <c r="O126">
+        <v>0.02</v>
+      </c>
+      <c r="P126">
+        <v>0.03</v>
+      </c>
+      <c r="Q126">
+        <v>0.04</v>
+      </c>
+      <c r="R126">
+        <v>0.04</v>
+      </c>
+      <c r="S126">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AD126">
+        <f>AVERAGE(B126:S126)</f>
+        <v>3.5555555555555562E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:30">
+      <c r="A129">
+        <f>A126+1</f>
+        <v>28</v>
+      </c>
+      <c r="B129">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C129">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D129">
+        <v>0.06</v>
+      </c>
+      <c r="E129">
+        <v>0.05</v>
+      </c>
+      <c r="F129">
+        <v>0.06</v>
+      </c>
+      <c r="G129">
+        <v>0.06</v>
+      </c>
+      <c r="H129">
+        <v>0.06</v>
+      </c>
+      <c r="I129">
+        <v>0.08</v>
+      </c>
+      <c r="J129">
+        <v>0.08</v>
+      </c>
+      <c r="K129">
+        <v>0.05</v>
+      </c>
+      <c r="L129">
+        <v>0.08</v>
+      </c>
+      <c r="M129">
+        <v>0.06</v>
+      </c>
+      <c r="N129">
+        <v>0.09</v>
+      </c>
+      <c r="AD129">
+        <f>AVERAGE(B129:N129)</f>
+        <v>6.6923076923076918E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:30">
+      <c r="A132">
+        <f>A129+1</f>
+        <v>29</v>
+      </c>
+      <c r="B132">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>0.11</v>
+      </c>
+      <c r="E132">
+        <v>0.05</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <v>0.09</v>
+      </c>
+      <c r="H132">
+        <v>0.03</v>
+      </c>
+      <c r="I132">
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <v>0.08</v>
+      </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M132">
+        <v>0.03</v>
+      </c>
+      <c r="N132">
+        <v>0.03</v>
+      </c>
+      <c r="O132">
+        <v>0.02</v>
+      </c>
+      <c r="P132">
+        <v>0.02</v>
+      </c>
+      <c r="Q132">
+        <v>0</v>
+      </c>
+      <c r="R132">
+        <v>0</v>
+      </c>
+      <c r="S132">
+        <v>0.02</v>
+      </c>
+      <c r="T132">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U132">
+        <v>0</v>
+      </c>
+      <c r="V132">
+        <v>0</v>
+      </c>
+      <c r="W132">
+        <v>0.02</v>
+      </c>
+      <c r="AD132">
+        <f>AVERAGE(B132:W132)</f>
+        <v>3.2272727272727279E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:30">
+      <c r="A135">
+        <f>A132+1</f>
+        <v>30</v>
+      </c>
+      <c r="B135">
+        <v>0.06</v>
+      </c>
+      <c r="C135">
+        <v>0.06</v>
+      </c>
+      <c r="D135">
+        <v>0.04</v>
+      </c>
+      <c r="E135">
+        <v>0.06</v>
+      </c>
+      <c r="F135">
+        <v>0.11</v>
+      </c>
+      <c r="G135">
+        <v>0.03</v>
+      </c>
+      <c r="H135">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I135">
+        <v>0.05</v>
+      </c>
+      <c r="J135">
+        <v>0.06</v>
+      </c>
+      <c r="K135">
+        <v>0.05</v>
+      </c>
+      <c r="L135">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M135">
+        <v>0.12</v>
+      </c>
+      <c r="N135">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O135">
+        <v>0.05</v>
+      </c>
+      <c r="P135">
+        <v>0.13</v>
+      </c>
+      <c r="AD135">
+        <f>AVERAGE(B135:P135)</f>
+        <v>7.3333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:30">
+      <c r="A138">
+        <f>A135+1</f>
+        <v>31</v>
+      </c>
+      <c r="B138">
+        <v>0.02</v>
+      </c>
+      <c r="C138">
+        <v>0.03</v>
+      </c>
+      <c r="D138">
+        <v>0.05</v>
+      </c>
+      <c r="E138">
+        <v>0.04</v>
+      </c>
+      <c r="F138">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G138">
+        <v>0.08</v>
+      </c>
+      <c r="H138">
+        <v>0.06</v>
+      </c>
+      <c r="I138">
+        <v>0.04</v>
+      </c>
+      <c r="J138">
+        <v>0.02</v>
+      </c>
+      <c r="K138">
+        <v>0.04</v>
+      </c>
+      <c r="L138">
+        <v>0.03</v>
+      </c>
+      <c r="M138">
+        <v>0.06</v>
+      </c>
+      <c r="N138">
+        <v>0.02</v>
+      </c>
+      <c r="O138">
+        <v>0.05</v>
+      </c>
+      <c r="P138">
+        <v>0.09</v>
+      </c>
+      <c r="Q138">
+        <v>0.06</v>
+      </c>
+      <c r="R138">
+        <v>0.1</v>
+      </c>
+      <c r="AD138">
+        <f>AVERAGE(B138:R138)</f>
+        <v>5.0588235294117649E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:30">
+      <c r="A141">
+        <f>A138+1</f>
+        <v>32</v>
+      </c>
+      <c r="B141">
+        <v>0.04</v>
+      </c>
+      <c r="C141">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D141">
+        <v>0.08</v>
+      </c>
+      <c r="E141">
+        <v>0.1</v>
+      </c>
+      <c r="F141">
+        <v>0.05</v>
+      </c>
+      <c r="G141">
+        <v>0.04</v>
+      </c>
+      <c r="H141">
+        <v>0.08</v>
+      </c>
+      <c r="I141">
+        <v>0.04</v>
+      </c>
+      <c r="J141">
+        <v>0.05</v>
+      </c>
+      <c r="K141">
+        <v>0.01</v>
+      </c>
+      <c r="L141">
+        <v>0.05</v>
+      </c>
+      <c r="AD141">
+        <f>AVERAGE(B141:L141)</f>
+        <v>5.5454545454545465E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:30">
+      <c r="A144">
+        <f>A141+1</f>
+        <v>33</v>
+      </c>
+      <c r="B144">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C144">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D144">
+        <v>0.11</v>
+      </c>
+      <c r="E144">
+        <v>0.1</v>
+      </c>
+      <c r="F144">
+        <v>0.08</v>
+      </c>
+      <c r="G144">
+        <v>0.1</v>
+      </c>
+      <c r="H144">
+        <v>0.08</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>0.04</v>
+      </c>
+      <c r="K144">
+        <v>0.09</v>
+      </c>
+      <c r="L144">
+        <v>0.11</v>
+      </c>
+      <c r="M144">
+        <v>0.1</v>
+      </c>
+      <c r="N144">
+        <v>0.02</v>
+      </c>
+      <c r="AD144">
+        <f>AVERAGE(B144:N144)</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="147" spans="1:30">
+      <c r="A147">
+        <f>A144+1</f>
+        <v>34</v>
+      </c>
+      <c r="B147">
+        <v>0.04</v>
+      </c>
+      <c r="C147">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>0.05</v>
+      </c>
+      <c r="G147">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H147">
+        <v>0.04</v>
+      </c>
+      <c r="I147">
+        <v>0.05</v>
+      </c>
+      <c r="J147">
+        <v>0.02</v>
+      </c>
+      <c r="K147">
+        <v>0.03</v>
+      </c>
+      <c r="L147">
+        <v>0.05</v>
+      </c>
+      <c r="M147">
+        <v>0.04</v>
+      </c>
+      <c r="N147">
+        <v>0.04</v>
+      </c>
+      <c r="O147">
+        <v>0.04</v>
+      </c>
+      <c r="P147">
+        <v>0.06</v>
+      </c>
+      <c r="Q147">
+        <v>0.02</v>
+      </c>
+      <c r="R147">
+        <v>0.03</v>
+      </c>
+      <c r="AD147">
+        <f>AVERAGE(B147:R147)</f>
+        <v>3.8235294117647055E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:30">
+      <c r="A150">
+        <f t="shared" ref="A150" si="1">A147+1</f>
+        <v>35</v>
+      </c>
+      <c r="B150">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C150">
+        <v>0.13</v>
+      </c>
+      <c r="D150">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E150">
+        <v>0.06</v>
+      </c>
+      <c r="F150">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G150">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>0.05</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150">
+        <v>0.03</v>
+      </c>
+      <c r="L150">
+        <v>0.08</v>
+      </c>
+      <c r="M150">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N150">
+        <v>0.12</v>
+      </c>
+      <c r="O150">
+        <v>0.01</v>
+      </c>
+      <c r="AD150">
+        <f>AVERAGE(B150:O150)</f>
+        <v>5.9285714285714282E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>